<commit_message>
added @DataProvider and second test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semay\IdeaProjects\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F6B0055-93F1-4990-8479-4A52FAED0882}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07F2E86-9A55-48F5-9470-1709E2C8089B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{46B9D7B7-BA71-4904-85EC-8A47F78EF0A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,6 +31,32 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Jonhson</t>
+  </si>
+  <si>
+    <t>fistName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>postCode</t>
+  </si>
+  <si>
+    <t>alertText</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,14 +406,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A309068-8F3B-407C-A3B8-0207767EE022}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>11230</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Extend Report and Custom DataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semay\IdeaProjects\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07F2E86-9A55-48F5-9470-1709E2C8089B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE81679-C0EB-4908-A3A0-794C2FD5CDFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{46B9D7B7-BA71-4904-85EC-8A47F78EF0A2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{46B9D7B7-BA71-4904-85EC-8A47F78EF0A2}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Alice</t>
   </si>
@@ -55,6 +56,18 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Alice Johnson</t>
+  </si>
+  <si>
+    <t>Dollar</t>
   </si>
 </sst>
 </file>
@@ -408,7 +421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A309068-8F3B-407C-A3B8-0207767EE022}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -445,4 +458,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527DD752-DAE6-4F3C-A4B2-94E18472ABAA}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test suite in excel and and in a test case run mode
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semay\IdeaProjects\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE81679-C0EB-4908-A3A0-794C2FD5CDFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847C8322-68E1-418D-BFD0-7F9F64F61F90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{46B9D7B7-BA71-4904-85EC-8A47F78EF0A2}"/>
+    <workbookView xWindow="3740" yWindow="2110" windowWidth="14400" windowHeight="7460" activeTab="2" xr2:uid="{46B9D7B7-BA71-4904-85EC-8A47F78EF0A2}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
     <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Alice</t>
   </si>
@@ -64,23 +65,71 @@
     <t>currency</t>
   </si>
   <si>
-    <t>Alice Johnson</t>
-  </si>
-  <si>
     <t>Dollar</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Gates</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Zukenberg</t>
+  </si>
+  <si>
+    <t>John Adam</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>rumode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,8 +152,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,15 +471,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A309068-8F3B-407C-A3B8-0207767EE022}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="24.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -440,8 +495,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -453,6 +511,60 @@
       </c>
       <c r="D2" t="s">
         <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>11235</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>11100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>12300</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -464,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527DD752-DAE6-4F3C-A4B2-94E18472ABAA}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,13 +595,64 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F4B5BD-97A3-46DB-A3D1-791208D8874B}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
set run modes and implemented parameters
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semay\IdeaProjects\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847C8322-68E1-418D-BFD0-7F9F64F61F90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F8AB96-C28A-4A08-9142-2BF3A54C3D01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="2110" windowWidth="14400" windowHeight="7460" activeTab="2" xr2:uid="{46B9D7B7-BA71-4904-85EC-8A47F78EF0A2}"/>
+    <workbookView xWindow="31410" yWindow="1995" windowWidth="14400" windowHeight="7455" xr2:uid="{46B9D7B7-BA71-4904-85EC-8A47F78EF0A2}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Alice</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Jonhson</t>
   </si>
   <si>
-    <t>fistName</t>
-  </si>
-  <si>
     <t>lastName</t>
   </si>
   <si>
@@ -110,7 +107,7 @@
     <t>runmode</t>
   </si>
   <si>
-    <t>rumode</t>
+    <t>firstName</t>
   </si>
 </sst>
 </file>
@@ -473,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A309068-8F3B-407C-A3B8-0207767EE022}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,19 +481,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -510,61 +507,61 @@
         <v>11230</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
       </c>
       <c r="C3">
         <v>11235</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
       </c>
       <c r="C4">
         <v>11100</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
       </c>
       <c r="C5">
         <v>12300</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -587,18 +584,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -610,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F4B5BD-97A3-46DB-A3D1-791208D8874B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,34 +618,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated chrome driver last version
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semay\IdeaProjects\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F8AB96-C28A-4A08-9142-2BF3A54C3D01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541733BC-11E5-4E78-94EB-B645E5714A0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31410" yWindow="1995" windowWidth="14400" windowHeight="7455" xr2:uid="{46B9D7B7-BA71-4904-85EC-8A47F78EF0A2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{46B9D7B7-BA71-4904-85EC-8A47F78EF0A2}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Alice</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>OpenAccountTest</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>runmode</t>
@@ -471,7 +468,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,7 +478,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -493,7 +490,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -544,7 +541,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -608,7 +605,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,7 +618,7 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>